<commit_message>
From 1.0 to 1.1 version
</commit_message>
<xml_diff>
--- a/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
+++ b/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
@@ -98,34 +98,34 @@
     <t>SYSTEM apresenta um formulario com campos de nome de usuario e senha e um botao entrar</t>
   </si>
   <si>
+    <t>Usuario do Sistema preenche os campos e clica no botao entrar</t>
+  </si>
+  <si>
+    <t>SYSTEM alerta que o CAS (sistema de autorizacao login-senha) esta fora do ar</t>
+  </si>
+  <si>
     <t>Usuario do Sistema seleciona um nome de usuario sugerido, digita a senha e clica no botao entrar</t>
   </si>
   <si>
+    <t>SYSTEM exibe uma mensagem de sucesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuario logado com sucesso</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
     <t>SYSTEM alerta que o TJSeg (sistema que fornece as permissoes de acesso e escrita) esta fora do ar</t>
   </si>
   <si>
-    <t>Usuario do Sistema preenche os campos e clica no botao entrar</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe uma mensagem de sucesso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuario logado com sucesso</t>
-  </si>
-  <si>
-    <t>TC2</t>
+    <t>TC3</t>
   </si>
   <si>
     <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>SYSTEM alerta que o CAS (sistema de autorizacao login-senha) esta fora do ar</t>
   </si>
 </sst>
 </file>
@@ -826,7 +826,7 @@
         <v>2.0</v>
       </c>
       <c r="B31" t="s" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s" s="6">
         <v>2</v>
@@ -846,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s" s="6">
         <v>2</v>

</xml_diff>

<commit_message>
From 1.1 to 1.2 version
</commit_message>
<xml_diff>
--- a/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
+++ b/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
@@ -119,13 +119,13 @@
     <t>TC2</t>
   </si>
   <si>
+    <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
     <t>SYSTEM alerta que o TJSeg (sistema que fornece as permissoes de acesso e escrita) esta fora do ar</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
         <v>2.0</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s" s="6">
         <v>2</v>

</xml_diff>

<commit_message>
From 1.2 to 1.3 version
</commit_message>
<xml_diff>
--- a/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
+++ b/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
@@ -98,34 +98,34 @@
     <t>SYSTEM apresenta um formulario com campos de nome de usuario e senha e um botao entrar</t>
   </si>
   <si>
+    <t>Usuario do Sistema seleciona um nome de usuario sugerido, digita a senha e clica no botao entrar</t>
+  </si>
+  <si>
+    <t>SYSTEM alerta que o TJSeg (sistema que fornece as permissoes de acesso e escrita) esta fora do ar</t>
+  </si>
+  <si>
     <t>Usuario do Sistema preenche os campos e clica no botao entrar</t>
   </si>
   <si>
+    <t>SYSTEM exibe uma mensagem de sucesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuario logado com sucesso</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
     <t>SYSTEM alerta que o CAS (sistema de autorizacao login-senha) esta fora do ar</t>
-  </si>
-  <si>
-    <t>Usuario do Sistema seleciona um nome de usuario sugerido, digita a senha e clica no botao entrar</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe uma mensagem de sucesso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuario logado com sucesso</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>SYSTEM alerta que o TJSeg (sistema que fornece as permissoes de acesso e escrita) esta fora do ar</t>
   </si>
 </sst>
 </file>
@@ -846,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s" s="6">
         <v>2</v>

</xml_diff>

<commit_message>
From 1.3 to 1.4 version
</commit_message>
<xml_diff>
--- a/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
+++ b/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
@@ -92,34 +92,34 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Usuario do Sistema inicia a tela de login atraves da opcao de Login no canto superior direito</t>
+    <t>Usuario do Sistema abre a tela de login atraves da opcao de Login no canto superior direito</t>
   </si>
   <si>
     <t>SYSTEM apresenta um formulario com campos de nome de usuario e senha e um botao entrar</t>
   </si>
   <si>
+    <t>Usuario do Sistema preenche os campos e clica no botao entrar</t>
+  </si>
+  <si>
+    <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
+  </si>
+  <si>
     <t>Usuario do Sistema seleciona um nome de usuario sugerido, digita a senha e clica no botao entrar</t>
   </si>
   <si>
+    <t>SYSTEM exibe uma mensagem de sucesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuario logado com sucesso</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
     <t>SYSTEM alerta que o TJSeg (sistema que fornece as permissoes de acesso e escrita) esta fora do ar</t>
-  </si>
-  <si>
-    <t>Usuario do Sistema preenche os campos e clica no botao entrar</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe uma mensagem de sucesso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuario logado com sucesso</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
   </si>
   <si>
     <t>TC3</t>
@@ -684,7 +684,7 @@
         <v>3.0</v>
       </c>
       <c r="B22" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s" s="6">
         <v>2</v>
@@ -846,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s" s="6">
         <v>2</v>

</xml_diff>

<commit_message>
From 1.4 to 1.5 version
</commit_message>
<xml_diff>
--- a/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
+++ b/output/xlsx/RF001 - Autenticar Usuario--GT-.xlsx
@@ -101,31 +101,31 @@
     <t>Usuario do Sistema preenche os campos e clica no botao entrar</t>
   </si>
   <si>
+    <t>SYSTEM alerta que o CAS (sistema de autorizacao login-senha) esta fora do ar</t>
+  </si>
+  <si>
+    <t>Usuario do Sistema seleciona um nome de usuario sugerido, digita a senha e clica no botao entrar</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe uma mensagem de sucesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuario logado com sucesso</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
     <t>SYSTEM alerta que o nome de usuario e/ou senha estao incorretos</t>
   </si>
   <si>
-    <t>Usuario do Sistema seleciona um nome de usuario sugerido, digita a senha e clica no botao entrar</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe uma mensagem de sucesso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuario logado com sucesso</t>
-  </si>
-  <si>
-    <t>TC2</t>
+    <t>TC3</t>
   </si>
   <si>
     <t>SYSTEM alerta que o TJSeg (sistema que fornece as permissoes de acesso e escrita) esta fora do ar</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>SYSTEM alerta que o CAS (sistema de autorizacao login-senha) esta fora do ar</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
         <v>3.0</v>
       </c>
       <c r="B22" t="s" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s" s="6">
         <v>2</v>
@@ -826,7 +826,7 @@
         <v>2.0</v>
       </c>
       <c r="B31" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s" s="6">
         <v>2</v>
@@ -846,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s" s="6">
         <v>2</v>

</xml_diff>